<commit_message>
Redesign Excel Overview and Adjust Code for Redesign
-Next: Start with transaction processing
</commit_message>
<xml_diff>
--- a/exe/Backup/Utilities.xlsx
+++ b/exe/Backup/Utilities.xlsx
@@ -1,38 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\Backup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006E1680-D015-44B1-9BDF-8EB798A34DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Properties</t>
   </si>
@@ -40,10 +22,10 @@
     <t>Current Row/Column</t>
   </si>
   <si>
-    <t>Wealth Class in Allocation Row</t>
-  </si>
-  <si>
-    <t>Wealth Class in Cash Flow Row</t>
+    <t>Current Income Row in IC Sheet</t>
+  </si>
+  <si>
+    <t>Current Expense Row in IC Sheet</t>
   </si>
   <si>
     <t>Account Row</t>
@@ -52,26 +34,20 @@
     <t>Wealth Row</t>
   </si>
   <si>
-    <t>Income Row</t>
-  </si>
-  <si>
-    <t>Expense Row</t>
-  </si>
-  <si>
     <t>Records Row</t>
   </si>
   <si>
     <t>Records Banks Column</t>
   </si>
   <si>
-    <t>K</t>
+    <t>G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,18 +80,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -381,16 +349,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,31 +364,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -430,7 +396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -438,28 +404,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>